<commit_message>
experiment: measure runtime with different pruning ratio
</commit_message>
<xml_diff>
--- a/split-resnet50/runtime.xlsx
+++ b/split-resnet50/runtime.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mejhg\OneDrive\Desktop\vscode\hetde\split-resnet50\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74704B0-78CB-4B33-B1E5-40E9B8A7433A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ACE4AB-F2B3-459F-A62A-EA886B1F5B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FDEB8DA6-1FC5-479B-B8DF-57B4320A394B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FDEB8DA6-1FC5-479B-B8DF-57B4320A394B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$B$26:$B$30</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$B$27:$B$30</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$C$26:$C$30</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$C$27:$C$30</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$B$26:$B$30</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$B$27:$B$30</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">Sheet1!$C$26:$C$30</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">Sheet1!$C$27:$C$30</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$C$26:$C$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>average</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,6 +120,26 @@
     <t>convolution 파트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>whole model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rpc에서 prune 90% 했을 때</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rpc에서 prune 100% 했을 때</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>network overhead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rpc에서 prune 아무것도 안 했을 때</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -169,9 +184,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1978,10 +1996,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v2.4</cx:f>
+        <cx:f>_xlchart.v2.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v2.6</cx:f>
+        <cx:f>_xlchart.v2.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4935,8 +4953,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3777910" y="5379274"/>
-              <a:ext cx="3899720" cy="2317782"/>
+              <a:off x="3795279" y="5029650"/>
+              <a:ext cx="3915168" cy="2172106"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5883,6 +5901,342 @@
             <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
             <a:t>?</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FABEEDB-059B-8C3A-DC28-3489BB667D62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5524500" y="3362325"/>
+          <a:ext cx="7467600" cy="4286250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>결과</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200"/>
+            <a:t>1. pruning 100%</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>와 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200"/>
+            <a:t>100%</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>가 아닌 것 사이의 속도 차이가 극심</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200"/>
+            <a:t>=&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200"/>
+            <a:t>아예 안 보내는건 엄청 빠른데 중간 부분만 골라서 보내는건 꽤 느린 것 같음</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>보낼 부분만 담긴 연속적인 바이트 배열이 필요하니까 분명 복사가 일어날거고 이게 메인 오버헤드일 가능성이 큼</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>2. pruning </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>아예 안 한게 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>90% </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>한 것보다 더 빠르게 나옴</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>=&gt; pruning 90% </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>버전이 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>pruning </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>없는 버전에 비해  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>network overhead </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>수치는 줄었지만 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>whole model </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>시간이 증가한 것은 워커 노드 쪽에서 계산하기 전에 텐서의 빈 공간을 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>0</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>으로 채워넣는 과정이 추가되어서 그런 것으로 추측함</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>실행 시간 측정할 때 요청 수신 직후부터는 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>computation</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>으로 취급하니까 입력 데이터를 원래 사이즈로 복원하는 과정도 여기에 들어감ㅇㅇ</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>표에 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>computation </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>수치도 기록했으면 좋았을텐데 필요 없을 줄 알고 그걸 빼먹었음</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>요약</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>pruning</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>하면 전송량 감소하는 것도 맞고 실제로 전송에 걸리는 시간도 미세하게 감소하지만</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>다음과 같은 작업이 추가로 필요해서 결국 빨라지지는 않음</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>:</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>1. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>중앙 서버</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t> - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>입력 데이터 중에서 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>unpruned </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>채널만 골라서 전송 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>메모리 할당 및 복사가 일어날 개연성이 무척 높음</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>2. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>워커 노드 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>수신한 입력 데이터는 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>unpruned </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>채널만 있으니 나머지 채널 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>0</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>으로 채워넣어 기존 입력 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
+            <a:t>shape</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" kern="1200" baseline="0"/>
+            <a:t>로 돌려놓기</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100" kern="1200" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6210,23 +6564,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F65D93-1273-4791-80D8-0F238ACB7A58}">
   <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G18" zoomScale="78" workbookViewId="0">
+    <sheetView topLeftCell="G18" zoomScale="78" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -6252,7 +6606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -6286,7 +6640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -6316,7 +6670,7 @@
         <v>9.9706000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -6346,7 +6700,7 @@
         <v>0.30342200000000003</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -6376,7 +6730,7 @@
         <v>0.64491600000000004</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="T6">
         <v>4</v>
       </c>
@@ -6384,7 +6738,7 @@
         <v>0.71432399999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -6398,7 +6752,7 @@
         <v>1.4188339999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -6412,7 +6766,7 @@
         <v>1.6344559999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -6426,7 +6780,7 @@
         <v>1.720672</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -6440,7 +6794,7 @@
         <v>1.7644139999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="T11">
         <v>9</v>
       </c>
@@ -6448,7 +6802,7 @@
         <v>2.4776790000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="T12">
         <v>10</v>
       </c>
@@ -6456,7 +6810,7 @@
         <v>2.6188370000000001</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
       <c r="T13">
         <v>11</v>
       </c>
@@ -6464,7 +6818,7 @@
         <v>2.7180520000000001</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="T14">
         <v>12</v>
       </c>
@@ -6472,7 +6826,7 @@
         <v>2.7958630000000002</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
       <c r="T15">
         <v>13</v>
       </c>
@@ -6480,7 +6834,7 @@
         <v>2.908903</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
       <c r="T16">
         <v>14</v>
       </c>
@@ -6488,7 +6842,7 @@
         <v>3.0179170000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>6</v>
       </c>
@@ -6517,7 +6871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -6549,7 +6903,7 @@
         <v>2.4083966626829154</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -6577,7 +6931,7 @@
         <v>0.34586532910664797</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -6605,7 +6959,7 @@
         <v>4.380683898925776E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>1</v>
       </c>
@@ -6633,7 +6987,7 @@
         <v>0.66843175888061457</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -6642,7 +6996,7 @@
         <v>0.66843175888061457</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -6650,7 +7004,7 @@
         <v>0.56518409999999997</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -6658,7 +7012,7 @@
         <v>0.50287389999999998</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>10</v>
       </c>
@@ -6666,13 +7020,203 @@
         <v>0.48479749999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30">
         <v>0.48067330000000003</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEC4F7D-E2ED-44DA-8685-24B9A43FCACA}">
+  <dimension ref="C6:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>0.86781940000000002</v>
+      </c>
+      <c r="E9">
+        <v>0.58698839999999997</v>
+      </c>
+      <c r="F9">
+        <v>0.86721539999999997</v>
+      </c>
+      <c r="G9">
+        <v>0.52155790000000002</v>
+      </c>
+      <c r="H9">
+        <v>0.67052279999999997</v>
+      </c>
+      <c r="I9">
+        <v>0.32862609999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>0.86559779999999997</v>
+      </c>
+      <c r="E10">
+        <v>0.57305969999999995</v>
+      </c>
+      <c r="F10">
+        <v>0.87797170000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.53927709999999995</v>
+      </c>
+      <c r="H10">
+        <v>0.63612089999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.30470710000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>0.84201380000000003</v>
+      </c>
+      <c r="E11">
+        <v>0.55580390000000002</v>
+      </c>
+      <c r="F11">
+        <v>0.88762459999999999</v>
+      </c>
+      <c r="G11">
+        <v>0.53346870000000002</v>
+      </c>
+      <c r="H11">
+        <v>0.66613370000000005</v>
+      </c>
+      <c r="I11">
+        <v>0.32912669999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>0.82799509999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.538991</v>
+      </c>
+      <c r="F12">
+        <v>0.85656790000000005</v>
+      </c>
+      <c r="G12">
+        <v>0.51393849999999996</v>
+      </c>
+      <c r="H12">
+        <v>0.67788459999999995</v>
+      </c>
+      <c r="I12">
+        <v>0.33770489999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>0.83914789999999995</v>
+      </c>
+      <c r="E13">
+        <v>0.55317519999999998</v>
+      </c>
+      <c r="F13">
+        <v>0.85463509999999998</v>
+      </c>
+      <c r="G13">
+        <v>0.51196229999999998</v>
+      </c>
+      <c r="H13">
+        <v>0.67352369999999995</v>
+      </c>
+      <c r="I13">
+        <v>0.3375611</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:E14" si="0">AVERAGE(D9:D13)</f>
+        <v>0.8485147999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.56160364000000007</v>
+      </c>
+      <c r="F14">
+        <f>AVERAGE(F9:F13)</f>
+        <v>0.86880293999999991</v>
+      </c>
+      <c r="G14">
+        <f>AVERAGE(G9:G13)</f>
+        <v>0.52404089999999992</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:I14" si="1">AVERAGE(H9:H13)</f>
+        <v>0.66483714000000005</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0.32754518000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>